<commit_message>
formato importacion usuarios actualizado
</commit_message>
<xml_diff>
--- a/public/uploads/users/formato-importacion-usuarios.xlsx
+++ b/public/uploads/users/formato-importacion-usuarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rirah\Desktop\TESIS\APOYOS\PROYECTO SERVIDOR\gestion-proyectos\public\Uploads\Recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SIGTG\public\uploads\users\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250A4F7B-90CB-480B-B9F3-C517A8348865}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="estudianteMateria" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <definedName name="roles_s">Roles!$A$3:$B$6</definedName>
     <definedName name="roles_se">Roles!$B$3:$C$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Nombre</t>
   </si>
   <si>
     <t>Administrador</t>
-  </si>
-  <si>
-    <t>Nombres</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
   </si>
   <si>
     <t>Docente</t>
@@ -81,32 +76,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">2- Solo seleccione valores de las </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>listas desplegables</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, otros valores no serán almacenados. </t>
-    </r>
-  </si>
-  <si>
     <t>usuario</t>
   </si>
   <si>
@@ -153,9 +122,6 @@
   </si>
   <si>
     <t>Escuela de Ingeniería Química y Alimentos</t>
-  </si>
-  <si>
-    <t>Codigo Materia</t>
   </si>
   <si>
     <t>codmateria</t>
@@ -434,32 +400,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">6-El </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CODIGO de MATERIA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> debe cumplir el Formato: ABC115, es decir, 3 letras y 3 numeros</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">7-Las letras que conforman el codigo de la materia deben ser ingresadas en </t>
     </r>
     <r>
@@ -569,37 +509,97 @@
     </r>
   </si>
   <si>
-    <t>Dennis Ernesto</t>
-  </si>
-  <si>
-    <t>Orellana Ramirez</t>
-  </si>
-  <si>
     <t>OR15012</t>
   </si>
   <si>
-    <t>Karla Maria</t>
-  </si>
-  <si>
     <t>AR14019</t>
   </si>
   <si>
-    <t>Abrego Reyes</t>
-  </si>
-  <si>
-    <t>PDM115</t>
-  </si>
-  <si>
     <t>Protocolo</t>
+  </si>
+  <si>
+    <t>Primer nombre</t>
+  </si>
+  <si>
+    <t>Segundo nombre</t>
+  </si>
+  <si>
+    <t>Primer apellido</t>
+  </si>
+  <si>
+    <t>Segundo apellido</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Ernesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karla </t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Orellana</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Abrego</t>
+  </si>
+  <si>
+    <t>Reyes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2- Seleccione los valores de las </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">listas desplegables </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ó escribala manualmente si la opción no se encuentra.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pasantía de Práctica Profesional</t>
+  </si>
+  <si>
+    <t>Trabajo de Investigación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -820,28 +820,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -850,13 +850,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -865,13 +865,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -882,13 +882,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -902,7 +902,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,104 +1217,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
-    <col min="4" max="6" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="28.25" customWidth="1"/>
-    <col min="8" max="9" width="42.875" customWidth="1"/>
+    <col min="1" max="2" width="19.625" customWidth="1"/>
+    <col min="3" max="4" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="28.25" customWidth="1"/>
+    <col min="9" max="9" width="73.25" customWidth="1"/>
+    <col min="10" max="10" width="42.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1321,11 +1337,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="23"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="23"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1333,11 +1350,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1345,11 +1363,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="2"/>
       <c r="I6" s="39"/>
-      <c r="J6" s="40"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1357,13 +1376,14 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+      <c r="I7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1371,13 +1391,14 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+      <c r="I8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1385,13 +1406,14 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="20"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1399,13 +1421,14 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="20"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1413,13 +1436,14 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="22"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1427,13 +1451,14 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+      <c r="I12" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1441,13 +1466,14 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="20"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1455,13 +1481,12 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="38"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1469,11 +1494,12 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1481,8 +1507,10 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="38"/>
+      <c r="I16" s="44"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1490,10 +1518,11 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="21"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1501,10 +1530,11 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1512,10 +1542,11 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1523,13 +1554,14 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1537,13 +1569,14 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="25"/>
-      <c r="J21" s="30"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+      <c r="I21" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1551,13 +1584,14 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="30"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="30"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1565,13 +1599,14 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1579,13 +1614,14 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="30"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="30"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1593,25 +1629,27 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="34"/>
-      <c r="J25" s="30"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="34"/>
+      <c r="K25" s="30"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="38"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="38"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="30"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="38"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="30"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1619,11 +1657,12 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="33"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1631,8 +1670,9 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1640,8 +1680,9 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1649,8 +1690,9 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1658,8 +1700,9 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1667,8 +1710,9 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1676,8 +1720,9 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1685,8 +1730,9 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1694,8 +1740,9 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1703,8 +1750,9 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1712,8 +1760,9 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1721,8 +1770,9 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1730,8 +1780,9 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1739,8 +1790,9 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1748,8 +1800,9 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1757,8 +1810,9 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1766,8 +1820,9 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1775,8 +1830,9 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1784,8 +1840,9 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1793,8 +1850,9 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1802,8 +1860,9 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1811,8 +1870,9 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1820,8 +1880,9 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1829,8 +1890,9 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1838,8 +1900,9 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1847,8 +1910,9 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1856,8 +1920,9 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1865,8 +1930,9 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1874,8 +1940,9 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1883,8 +1950,9 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1892,8 +1960,9 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1901,8 +1970,9 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1910,8 +1980,9 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1919,8 +1990,9 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1928,8 +2000,9 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1937,8 +2010,9 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1946,8 +2020,9 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1955,8 +2030,9 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1964,8 +2040,9 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1973,8 +2050,9 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1982,8 +2060,9 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1991,8 +2070,9 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2000,8 +2080,9 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2009,8 +2090,9 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2018,8 +2100,9 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2027,8 +2110,9 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2036,8 +2120,9 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2045,8 +2130,9 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2054,8 +2140,9 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2063,8 +2150,9 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2072,8 +2160,9 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2081,8 +2170,9 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2090,8 +2180,9 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2099,8 +2190,9 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2108,8 +2200,9 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2117,8 +2210,9 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2126,8 +2220,9 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2135,8 +2230,9 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2144,8 +2240,9 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2153,8 +2250,9 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2162,8 +2260,9 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2171,8 +2270,9 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2180,8 +2280,9 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2189,8 +2290,9 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2198,8 +2300,9 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2207,8 +2310,9 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2216,8 +2320,9 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2225,8 +2330,9 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2234,8 +2340,9 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2243,8 +2350,9 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2252,8 +2360,9 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2261,8 +2370,9 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2270,8 +2380,9 @@
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2279,8 +2390,9 @@
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2288,34 +2400,35 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="El codigo ingresado no cumple con el formato definido ABC123" promptTitle="Codigo Materia" prompt="Ingrese el Codigo de la Asignatura bajo el formato ABC123" sqref="D2:D101">
-      <formula1>IF(AND(LEN(MID(D2,1,LEN(D2)-3))=3,ISTEXT(+MID(D2,1,3)),LEN(MID(D2,4,LEN(D2)-3))=3,ISNUMBER(VALUE(MID(D2,4,3)))),TRUE,FALSE)</formula1>
+  <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Apellidos" prompt="Ingrese los Apellidos en el siguiente orden Apellido1 Apellido2" sqref="C2:D101" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nombres" prompt="Ingrese los Nombres en el siguiente orden Nombre1 Nombre2" sqref="A2:B101" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debe ingresar un carnet con el formato AB12345" promptTitle="Carnet" prompt="Formato de Carnet: AB12345" sqref="E2 E4:E101" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>IF(AND(LEN(MID(E2,1,LEN(E2)-5))=2,ISTEXT(+MID(E2,1,2)),LEN(MID(E2,3,LEN(E2)-2))=5,ISNUMBER(VALUE(MID(E2,3,5)))),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Apellidos" prompt="Ingrese los Apellidos en el siguiente orden Apellido1 Apellido2" sqref="B2:B101"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nombres" prompt="Ingrese los Nombres en el siguiente orden Nombre1 Nombre2" sqref="A2:A101"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debe ingresar un carnet con el formato AB12345" promptTitle="Carnet" prompt="Formato de Carnet: AB12345" sqref="C2 C4:C101">
-      <formula1>IF(AND(LEN(MID(C2,1,LEN(C2)-5))=2,ISTEXT(+MID(C2,1,2)),LEN(MID(C2,3,LEN(C2)-2))=5,ISNUMBER(VALUE(MID(C2,3,5)))),TRUE,FALSE)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Modalidad" prompt="Elige una opción de la lista" sqref="F1:F1048576" xr:uid="{9A308A54-517B-4BCD-A9E7-6EA2A988F000}">
+      <formula1>"Presencial,En línea"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Protocolo" prompt="Elija una opción de la lista, o escríbala manualmente" sqref="G1:G1048576" xr:uid="{99F1E5E0-8340-428A-8BBE-066E6E392C27}">
+      <formula1>"Trabajo de Investigación,Pasantía de Práctica Profesional,Pasantía de Investigación,Cursos de Especialización,Examen General Técnico Profesional"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lista de Escuelas" prompt="Seleccione una Escuela si el usuario a ingresar es nuevo" sqref="H1" xr:uid="{1B3D7765-1AEB-47EE-8AC7-FAA81FCCD7C4}">
+      <formula1>"Escuela de Arquitectura,Escuela de Ingeniería Mecánica,Escuela de Ingeniería Civil,Escuela de Ingeniería Eléctrica,Escuela de Ingeniería Industrial,Escuela de Ingeniería Química y de Ingeniería de Alimentos,Escuela de Ingeniería Sistemas Informaticos"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lista de Escuelas" prompt="Seleccione una Escuela si el usuario a ingresar es nuevo">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lista de Escuelas" prompt="Seleccione una Escuela si el usuario a ingresar es nuevo" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>Roles!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G101</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debe Seleccionar una de las dos Opciones" promptTitle="Modalidad Materia" prompt="Seleccione la Modalidad de la Materia">
-          <x14:formula1>
-            <xm:f>Roles!$H$2:$H$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:F101</xm:sqref>
+          <xm:sqref>H2:H101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2324,7 +2437,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2345,19 +2458,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2371,16 +2484,16 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2388,22 +2501,22 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2411,13 +2524,13 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -2428,13 +2541,13 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="8">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -2445,13 +2558,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="8">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -2462,13 +2575,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="8">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -2476,7 +2589,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -2489,7 +2602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2508,77 +2621,77 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>IF(estudianteMateria!$A2="","",estudianteMateria!$A2)</f>
-        <v>Dennis Ernesto</v>
+        <v>Dennis</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>IF(estudianteMateria!$B2="","",estudianteMateria!$B2)</f>
-        <v>Orellana Ramirez</v>
+        <f>IF(estudianteMateria!$C2="","",estudianteMateria!$C2)</f>
+        <v>Orellana</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>IF(estudianteMateria!$C2="","",estudianteMateria!$C2)</f>
+        <f>IF(estudianteMateria!$E2="","",estudianteMateria!$E2)</f>
         <v>OR15012</v>
       </c>
-      <c r="D2" s="2" t="str">
-        <f>IF(estudianteMateria!$D2="","",estudianteMateria!$D2)</f>
-        <v>PDM115</v>
+      <c r="D2" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E2,mod,2,FALSE),"")</f>
-        <v>L</v>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F2,mod,2,FALSE),"")</f>
+        <v>P</v>
       </c>
       <c r="F2" s="4">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G2,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H2,escuelas,2,FALSE),"")</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>IF(estudianteMateria!$A3="","",estudianteMateria!$A3)</f>
-        <v>Karla Maria</v>
+        <v xml:space="preserve">Karla </v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>IF(estudianteMateria!$B3="","",estudianteMateria!$B3)</f>
-        <v>Abrego Reyes</v>
+        <f>IF(estudianteMateria!$C3="","",estudianteMateria!$C3)</f>
+        <v>Abrego</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>IF(estudianteMateria!$C3="","",estudianteMateria!$C3)</f>
+        <f>IF(estudianteMateria!$E3="","",estudianteMateria!$E3)</f>
         <v>AR14019</v>
       </c>
-      <c r="D3" s="2" t="str">
-        <f>IF(estudianteMateria!$D3="","",estudianteMateria!$D3)</f>
-        <v>PDM115</v>
+      <c r="D3" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E3,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F3,mod,2,FALSE),"")</f>
         <v>P</v>
       </c>
       <c r="F3" s="4">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G3,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H3,escuelas,2,FALSE),"")</f>
         <v>1</v>
       </c>
     </row>
@@ -2588,23 +2701,23 @@
         <v/>
       </c>
       <c r="B4" s="2" t="str">
-        <f>IF(estudianteMateria!$B4="","",estudianteMateria!$B4)</f>
+        <f>IF(estudianteMateria!$C4="","",estudianteMateria!$C4)</f>
         <v/>
       </c>
       <c r="C4" s="2" t="str">
-        <f>IF(estudianteMateria!$C4="","",estudianteMateria!$C4)</f>
-        <v/>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>IF(estudianteMateria!$D4="","",estudianteMateria!$D4)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E4="","",estudianteMateria!$E4)</f>
+        <v/>
+      </c>
+      <c r="D4" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E4" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E4,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F4,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F4" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G4,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H4,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2614,23 +2727,23 @@
         <v/>
       </c>
       <c r="B5" s="2" t="str">
-        <f>IF(estudianteMateria!$B5="","",estudianteMateria!$B5)</f>
+        <f>IF(estudianteMateria!$C5="","",estudianteMateria!$C5)</f>
         <v/>
       </c>
       <c r="C5" s="2" t="str">
-        <f>IF(estudianteMateria!$C5="","",estudianteMateria!$C5)</f>
-        <v/>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f>IF(estudianteMateria!$D5="","",estudianteMateria!$D5)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E5="","",estudianteMateria!$E5)</f>
+        <v/>
+      </c>
+      <c r="D5" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E5,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F5,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F5" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G5,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H5,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2640,23 +2753,23 @@
         <v/>
       </c>
       <c r="B6" s="2" t="str">
-        <f>IF(estudianteMateria!$B6="","",estudianteMateria!$B6)</f>
+        <f>IF(estudianteMateria!$C6="","",estudianteMateria!$C6)</f>
         <v/>
       </c>
       <c r="C6" s="2" t="str">
-        <f>IF(estudianteMateria!$C6="","",estudianteMateria!$C6)</f>
-        <v/>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f>IF(estudianteMateria!$D6="","",estudianteMateria!$D6)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E6="","",estudianteMateria!$E6)</f>
+        <v/>
+      </c>
+      <c r="D6" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E6,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F6,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F6" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G6,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H6,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2666,23 +2779,23 @@
         <v/>
       </c>
       <c r="B7" s="2" t="str">
-        <f>IF(estudianteMateria!$B7="","",estudianteMateria!$B7)</f>
+        <f>IF(estudianteMateria!$C7="","",estudianteMateria!$C7)</f>
         <v/>
       </c>
       <c r="C7" s="2" t="str">
-        <f>IF(estudianteMateria!$C7="","",estudianteMateria!$C7)</f>
-        <v/>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f>IF(estudianteMateria!$D7="","",estudianteMateria!$D7)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E7="","",estudianteMateria!$E7)</f>
+        <v/>
+      </c>
+      <c r="D7" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E7,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F7,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F7" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G7,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H7,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2692,23 +2805,23 @@
         <v/>
       </c>
       <c r="B8" s="2" t="str">
-        <f>IF(estudianteMateria!$B8="","",estudianteMateria!$B8)</f>
+        <f>IF(estudianteMateria!$C8="","",estudianteMateria!$C8)</f>
         <v/>
       </c>
       <c r="C8" s="2" t="str">
-        <f>IF(estudianteMateria!$C8="","",estudianteMateria!$C8)</f>
-        <v/>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f>IF(estudianteMateria!$D8="","",estudianteMateria!$D8)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E8="","",estudianteMateria!$E8)</f>
+        <v/>
+      </c>
+      <c r="D8" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E8,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F8,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F8" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G8,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H8,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2718,23 +2831,23 @@
         <v/>
       </c>
       <c r="B9" s="2" t="str">
-        <f>IF(estudianteMateria!$B9="","",estudianteMateria!$B9)</f>
+        <f>IF(estudianteMateria!$C9="","",estudianteMateria!$C9)</f>
         <v/>
       </c>
       <c r="C9" s="2" t="str">
-        <f>IF(estudianteMateria!$C9="","",estudianteMateria!$C9)</f>
-        <v/>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f>IF(estudianteMateria!$D9="","",estudianteMateria!$D9)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E9="","",estudianteMateria!$E9)</f>
+        <v/>
+      </c>
+      <c r="D9" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E9,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F9,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F9" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G9,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H9,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2744,23 +2857,23 @@
         <v/>
       </c>
       <c r="B10" s="2" t="str">
-        <f>IF(estudianteMateria!$B10="","",estudianteMateria!$B10)</f>
+        <f>IF(estudianteMateria!$C10="","",estudianteMateria!$C10)</f>
         <v/>
       </c>
       <c r="C10" s="2" t="str">
-        <f>IF(estudianteMateria!$C10="","",estudianteMateria!$C10)</f>
-        <v/>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f>IF(estudianteMateria!$D10="","",estudianteMateria!$D10)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E10="","",estudianteMateria!$E10)</f>
+        <v/>
+      </c>
+      <c r="D10" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E10,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F10,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G10,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H10,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2770,23 +2883,23 @@
         <v/>
       </c>
       <c r="B11" s="2" t="str">
-        <f>IF(estudianteMateria!$B11="","",estudianteMateria!$B11)</f>
+        <f>IF(estudianteMateria!$C11="","",estudianteMateria!$C11)</f>
         <v/>
       </c>
       <c r="C11" s="2" t="str">
-        <f>IF(estudianteMateria!$C11="","",estudianteMateria!$C11)</f>
-        <v/>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f>IF(estudianteMateria!$D11="","",estudianteMateria!$D11)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E11="","",estudianteMateria!$E11)</f>
+        <v/>
+      </c>
+      <c r="D11" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E11,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F11,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F11" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G11,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H11,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2796,23 +2909,23 @@
         <v/>
       </c>
       <c r="B12" s="2" t="str">
-        <f>IF(estudianteMateria!$B12="","",estudianteMateria!$B12)</f>
+        <f>IF(estudianteMateria!$C12="","",estudianteMateria!$C12)</f>
         <v/>
       </c>
       <c r="C12" s="2" t="str">
-        <f>IF(estudianteMateria!$C12="","",estudianteMateria!$C12)</f>
-        <v/>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f>IF(estudianteMateria!$D12="","",estudianteMateria!$D12)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E12="","",estudianteMateria!$E12)</f>
+        <v/>
+      </c>
+      <c r="D12" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E12,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F12,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G12,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H12,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2822,23 +2935,23 @@
         <v/>
       </c>
       <c r="B13" s="2" t="str">
-        <f>IF(estudianteMateria!$B13="","",estudianteMateria!$B13)</f>
+        <f>IF(estudianteMateria!$C13="","",estudianteMateria!$C13)</f>
         <v/>
       </c>
       <c r="C13" s="2" t="str">
-        <f>IF(estudianteMateria!$C13="","",estudianteMateria!$C13)</f>
-        <v/>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f>IF(estudianteMateria!$D13="","",estudianteMateria!$D13)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E13="","",estudianteMateria!$E13)</f>
+        <v/>
+      </c>
+      <c r="D13" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E13,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F13,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F13" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G13,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H13,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2848,23 +2961,23 @@
         <v/>
       </c>
       <c r="B14" s="2" t="str">
-        <f>IF(estudianteMateria!$B14="","",estudianteMateria!$B14)</f>
+        <f>IF(estudianteMateria!$C14="","",estudianteMateria!$C14)</f>
         <v/>
       </c>
       <c r="C14" s="2" t="str">
-        <f>IF(estudianteMateria!$C14="","",estudianteMateria!$C14)</f>
-        <v/>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f>IF(estudianteMateria!$D14="","",estudianteMateria!$D14)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E14="","",estudianteMateria!$E14)</f>
+        <v/>
+      </c>
+      <c r="D14" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E14,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F14,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F14" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G14,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H14,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2874,23 +2987,23 @@
         <v/>
       </c>
       <c r="B15" s="2" t="str">
-        <f>IF(estudianteMateria!$B15="","",estudianteMateria!$B15)</f>
+        <f>IF(estudianteMateria!$C15="","",estudianteMateria!$C15)</f>
         <v/>
       </c>
       <c r="C15" s="2" t="str">
-        <f>IF(estudianteMateria!$C15="","",estudianteMateria!$C15)</f>
-        <v/>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f>IF(estudianteMateria!$D15="","",estudianteMateria!$D15)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E15="","",estudianteMateria!$E15)</f>
+        <v/>
+      </c>
+      <c r="D15" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E15,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F15,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F15" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G15,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H15,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2900,23 +3013,23 @@
         <v/>
       </c>
       <c r="B16" s="2" t="str">
-        <f>IF(estudianteMateria!$B16="","",estudianteMateria!$B16)</f>
+        <f>IF(estudianteMateria!$C16="","",estudianteMateria!$C16)</f>
         <v/>
       </c>
       <c r="C16" s="2" t="str">
-        <f>IF(estudianteMateria!$C16="","",estudianteMateria!$C16)</f>
-        <v/>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f>IF(estudianteMateria!$D16="","",estudianteMateria!$D16)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E16="","",estudianteMateria!$E16)</f>
+        <v/>
+      </c>
+      <c r="D16" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E16,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F16,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F16" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G16,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H16,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2926,23 +3039,23 @@
         <v/>
       </c>
       <c r="B17" s="2" t="str">
-        <f>IF(estudianteMateria!$B17="","",estudianteMateria!$B17)</f>
+        <f>IF(estudianteMateria!$C17="","",estudianteMateria!$C17)</f>
         <v/>
       </c>
       <c r="C17" s="2" t="str">
-        <f>IF(estudianteMateria!$C17="","",estudianteMateria!$C17)</f>
-        <v/>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f>IF(estudianteMateria!$D17="","",estudianteMateria!$D17)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E17="","",estudianteMateria!$E17)</f>
+        <v/>
+      </c>
+      <c r="D17" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E17,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F17,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F17" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G17,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H17,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2952,23 +3065,23 @@
         <v/>
       </c>
       <c r="B18" s="2" t="str">
-        <f>IF(estudianteMateria!$B18="","",estudianteMateria!$B18)</f>
+        <f>IF(estudianteMateria!$C18="","",estudianteMateria!$C18)</f>
         <v/>
       </c>
       <c r="C18" s="2" t="str">
-        <f>IF(estudianteMateria!$C18="","",estudianteMateria!$C18)</f>
-        <v/>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f>IF(estudianteMateria!$D18="","",estudianteMateria!$D18)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E18="","",estudianteMateria!$E18)</f>
+        <v/>
+      </c>
+      <c r="D18" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E18,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F18,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F18" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G18,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H18,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -2978,23 +3091,23 @@
         <v/>
       </c>
       <c r="B19" s="2" t="str">
-        <f>IF(estudianteMateria!$B19="","",estudianteMateria!$B19)</f>
+        <f>IF(estudianteMateria!$C19="","",estudianteMateria!$C19)</f>
         <v/>
       </c>
       <c r="C19" s="2" t="str">
-        <f>IF(estudianteMateria!$C19="","",estudianteMateria!$C19)</f>
-        <v/>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>IF(estudianteMateria!$D19="","",estudianteMateria!$D19)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E19="","",estudianteMateria!$E19)</f>
+        <v/>
+      </c>
+      <c r="D19" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E19,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F19,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F19" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G19,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H19,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3004,23 +3117,23 @@
         <v/>
       </c>
       <c r="B20" s="2" t="str">
-        <f>IF(estudianteMateria!$B20="","",estudianteMateria!$B20)</f>
+        <f>IF(estudianteMateria!$C20="","",estudianteMateria!$C20)</f>
         <v/>
       </c>
       <c r="C20" s="2" t="str">
-        <f>IF(estudianteMateria!$C20="","",estudianteMateria!$C20)</f>
-        <v/>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>IF(estudianteMateria!$D20="","",estudianteMateria!$D20)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E20="","",estudianteMateria!$E20)</f>
+        <v/>
+      </c>
+      <c r="D20" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E20,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F20,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F20" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G20,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H20,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3030,23 +3143,23 @@
         <v/>
       </c>
       <c r="B21" s="2" t="str">
-        <f>IF(estudianteMateria!$B21="","",estudianteMateria!$B21)</f>
+        <f>IF(estudianteMateria!$C21="","",estudianteMateria!$C21)</f>
         <v/>
       </c>
       <c r="C21" s="2" t="str">
-        <f>IF(estudianteMateria!$C21="","",estudianteMateria!$C21)</f>
-        <v/>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f>IF(estudianteMateria!$D21="","",estudianteMateria!$D21)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E21="","",estudianteMateria!$E21)</f>
+        <v/>
+      </c>
+      <c r="D21" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E21,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F21,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F21" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G21,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H21,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3056,23 +3169,23 @@
         <v/>
       </c>
       <c r="B22" s="2" t="str">
-        <f>IF(estudianteMateria!$B22="","",estudianteMateria!$B22)</f>
+        <f>IF(estudianteMateria!$C22="","",estudianteMateria!$C22)</f>
         <v/>
       </c>
       <c r="C22" s="2" t="str">
-        <f>IF(estudianteMateria!$C22="","",estudianteMateria!$C22)</f>
-        <v/>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f>IF(estudianteMateria!$D22="","",estudianteMateria!$D22)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E22="","",estudianteMateria!$E22)</f>
+        <v/>
+      </c>
+      <c r="D22" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E22,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F22,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F22" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G22,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H22,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3082,23 +3195,23 @@
         <v/>
       </c>
       <c r="B23" s="2" t="str">
-        <f>IF(estudianteMateria!$B23="","",estudianteMateria!$B23)</f>
+        <f>IF(estudianteMateria!$C23="","",estudianteMateria!$C23)</f>
         <v/>
       </c>
       <c r="C23" s="2" t="str">
-        <f>IF(estudianteMateria!$C23="","",estudianteMateria!$C23)</f>
-        <v/>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f>IF(estudianteMateria!$D23="","",estudianteMateria!$D23)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E23="","",estudianteMateria!$E23)</f>
+        <v/>
+      </c>
+      <c r="D23" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E23,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F23,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F23" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G23,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H23,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3108,23 +3221,23 @@
         <v/>
       </c>
       <c r="B24" s="2" t="str">
-        <f>IF(estudianteMateria!$B24="","",estudianteMateria!$B24)</f>
+        <f>IF(estudianteMateria!$C24="","",estudianteMateria!$C24)</f>
         <v/>
       </c>
       <c r="C24" s="2" t="str">
-        <f>IF(estudianteMateria!$C24="","",estudianteMateria!$C24)</f>
-        <v/>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f>IF(estudianteMateria!$D24="","",estudianteMateria!$D24)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E24="","",estudianteMateria!$E24)</f>
+        <v/>
+      </c>
+      <c r="D24" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E24,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F24,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F24" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G24,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H24,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3134,23 +3247,23 @@
         <v/>
       </c>
       <c r="B25" s="2" t="str">
-        <f>IF(estudianteMateria!$B25="","",estudianteMateria!$B25)</f>
+        <f>IF(estudianteMateria!$C25="","",estudianteMateria!$C25)</f>
         <v/>
       </c>
       <c r="C25" s="2" t="str">
-        <f>IF(estudianteMateria!$C25="","",estudianteMateria!$C25)</f>
-        <v/>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f>IF(estudianteMateria!$D25="","",estudianteMateria!$D25)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E25="","",estudianteMateria!$E25)</f>
+        <v/>
+      </c>
+      <c r="D25" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E25,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F25,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F25" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G25,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H25,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3160,23 +3273,23 @@
         <v/>
       </c>
       <c r="B26" s="2" t="str">
-        <f>IF(estudianteMateria!$B26="","",estudianteMateria!$B26)</f>
+        <f>IF(estudianteMateria!$C26="","",estudianteMateria!$C26)</f>
         <v/>
       </c>
       <c r="C26" s="2" t="str">
-        <f>IF(estudianteMateria!$C26="","",estudianteMateria!$C26)</f>
-        <v/>
-      </c>
-      <c r="D26" s="2" t="str">
-        <f>IF(estudianteMateria!$D26="","",estudianteMateria!$D26)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E26="","",estudianteMateria!$E26)</f>
+        <v/>
+      </c>
+      <c r="D26" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E26,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F26,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F26" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G26,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H26,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3186,23 +3299,23 @@
         <v/>
       </c>
       <c r="B27" s="2" t="str">
-        <f>IF(estudianteMateria!$B27="","",estudianteMateria!$B27)</f>
+        <f>IF(estudianteMateria!$C27="","",estudianteMateria!$C27)</f>
         <v/>
       </c>
       <c r="C27" s="2" t="str">
-        <f>IF(estudianteMateria!$C27="","",estudianteMateria!$C27)</f>
-        <v/>
-      </c>
-      <c r="D27" s="2" t="str">
-        <f>IF(estudianteMateria!$D27="","",estudianteMateria!$D27)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E27="","",estudianteMateria!$E27)</f>
+        <v/>
+      </c>
+      <c r="D27" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E27,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F27,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F27" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G27,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H27,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3212,23 +3325,23 @@
         <v/>
       </c>
       <c r="B28" s="2" t="str">
-        <f>IF(estudianteMateria!$B28="","",estudianteMateria!$B28)</f>
+        <f>IF(estudianteMateria!$C28="","",estudianteMateria!$C28)</f>
         <v/>
       </c>
       <c r="C28" s="2" t="str">
-        <f>IF(estudianteMateria!$C28="","",estudianteMateria!$C28)</f>
-        <v/>
-      </c>
-      <c r="D28" s="2" t="str">
-        <f>IF(estudianteMateria!$D28="","",estudianteMateria!$D28)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E28="","",estudianteMateria!$E28)</f>
+        <v/>
+      </c>
+      <c r="D28" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E28,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F28,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F28" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G28,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H28,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3238,23 +3351,23 @@
         <v/>
       </c>
       <c r="B29" s="2" t="str">
-        <f>IF(estudianteMateria!$B29="","",estudianteMateria!$B29)</f>
+        <f>IF(estudianteMateria!$C29="","",estudianteMateria!$C29)</f>
         <v/>
       </c>
       <c r="C29" s="2" t="str">
-        <f>IF(estudianteMateria!$C29="","",estudianteMateria!$C29)</f>
-        <v/>
-      </c>
-      <c r="D29" s="2" t="str">
-        <f>IF(estudianteMateria!$D29="","",estudianteMateria!$D29)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E29="","",estudianteMateria!$E29)</f>
+        <v/>
+      </c>
+      <c r="D29" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E29,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F29,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F29" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G29,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H29,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3264,23 +3377,23 @@
         <v/>
       </c>
       <c r="B30" s="2" t="str">
-        <f>IF(estudianteMateria!$B30="","",estudianteMateria!$B30)</f>
+        <f>IF(estudianteMateria!$C30="","",estudianteMateria!$C30)</f>
         <v/>
       </c>
       <c r="C30" s="2" t="str">
-        <f>IF(estudianteMateria!$C30="","",estudianteMateria!$C30)</f>
-        <v/>
-      </c>
-      <c r="D30" s="2" t="str">
-        <f>IF(estudianteMateria!$D30="","",estudianteMateria!$D30)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E30="","",estudianteMateria!$E30)</f>
+        <v/>
+      </c>
+      <c r="D30" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E30" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E30,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F30,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F30" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G30,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H30,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3290,23 +3403,23 @@
         <v/>
       </c>
       <c r="B31" s="2" t="str">
-        <f>IF(estudianteMateria!$B31="","",estudianteMateria!$B31)</f>
+        <f>IF(estudianteMateria!$C31="","",estudianteMateria!$C31)</f>
         <v/>
       </c>
       <c r="C31" s="2" t="str">
-        <f>IF(estudianteMateria!$C31="","",estudianteMateria!$C31)</f>
-        <v/>
-      </c>
-      <c r="D31" s="2" t="str">
-        <f>IF(estudianteMateria!$D31="","",estudianteMateria!$D31)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E31="","",estudianteMateria!$E31)</f>
+        <v/>
+      </c>
+      <c r="D31" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E31" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E31,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F31,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F31" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G31,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H31,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3316,23 +3429,23 @@
         <v/>
       </c>
       <c r="B32" s="2" t="str">
-        <f>IF(estudianteMateria!$B32="","",estudianteMateria!$B32)</f>
+        <f>IF(estudianteMateria!$C32="","",estudianteMateria!$C32)</f>
         <v/>
       </c>
       <c r="C32" s="2" t="str">
-        <f>IF(estudianteMateria!$C32="","",estudianteMateria!$C32)</f>
-        <v/>
-      </c>
-      <c r="D32" s="2" t="str">
-        <f>IF(estudianteMateria!$D32="","",estudianteMateria!$D32)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E32="","",estudianteMateria!$E32)</f>
+        <v/>
+      </c>
+      <c r="D32" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E32" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E32,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F32,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F32" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G32,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H32,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3342,23 +3455,23 @@
         <v/>
       </c>
       <c r="B33" s="2" t="str">
-        <f>IF(estudianteMateria!$B33="","",estudianteMateria!$B33)</f>
+        <f>IF(estudianteMateria!$C33="","",estudianteMateria!$C33)</f>
         <v/>
       </c>
       <c r="C33" s="2" t="str">
-        <f>IF(estudianteMateria!$C33="","",estudianteMateria!$C33)</f>
-        <v/>
-      </c>
-      <c r="D33" s="2" t="str">
-        <f>IF(estudianteMateria!$D33="","",estudianteMateria!$D33)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E33="","",estudianteMateria!$E33)</f>
+        <v/>
+      </c>
+      <c r="D33" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E33" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E33,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F33,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F33" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G33,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H33,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3368,23 +3481,23 @@
         <v/>
       </c>
       <c r="B34" s="2" t="str">
-        <f>IF(estudianteMateria!$B34="","",estudianteMateria!$B34)</f>
+        <f>IF(estudianteMateria!$C34="","",estudianteMateria!$C34)</f>
         <v/>
       </c>
       <c r="C34" s="2" t="str">
-        <f>IF(estudianteMateria!$C34="","",estudianteMateria!$C34)</f>
-        <v/>
-      </c>
-      <c r="D34" s="2" t="str">
-        <f>IF(estudianteMateria!$D34="","",estudianteMateria!$D34)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E34="","",estudianteMateria!$E34)</f>
+        <v/>
+      </c>
+      <c r="D34" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E34" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E34,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F34,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F34" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G34,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H34,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3394,23 +3507,23 @@
         <v/>
       </c>
       <c r="B35" s="2" t="str">
-        <f>IF(estudianteMateria!$B35="","",estudianteMateria!$B35)</f>
+        <f>IF(estudianteMateria!$C35="","",estudianteMateria!$C35)</f>
         <v/>
       </c>
       <c r="C35" s="2" t="str">
-        <f>IF(estudianteMateria!$C35="","",estudianteMateria!$C35)</f>
-        <v/>
-      </c>
-      <c r="D35" s="2" t="str">
-        <f>IF(estudianteMateria!$D35="","",estudianteMateria!$D35)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E35="","",estudianteMateria!$E35)</f>
+        <v/>
+      </c>
+      <c r="D35" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E35" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E35,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F35,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F35" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G35,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H35,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3420,23 +3533,23 @@
         <v/>
       </c>
       <c r="B36" s="2" t="str">
-        <f>IF(estudianteMateria!$B36="","",estudianteMateria!$B36)</f>
+        <f>IF(estudianteMateria!$C36="","",estudianteMateria!$C36)</f>
         <v/>
       </c>
       <c r="C36" s="2" t="str">
-        <f>IF(estudianteMateria!$C36="","",estudianteMateria!$C36)</f>
-        <v/>
-      </c>
-      <c r="D36" s="2" t="str">
-        <f>IF(estudianteMateria!$D36="","",estudianteMateria!$D36)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E36="","",estudianteMateria!$E36)</f>
+        <v/>
+      </c>
+      <c r="D36" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E36" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E36,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F36,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F36" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G36,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H36,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3446,23 +3559,23 @@
         <v/>
       </c>
       <c r="B37" s="2" t="str">
-        <f>IF(estudianteMateria!$B37="","",estudianteMateria!$B37)</f>
+        <f>IF(estudianteMateria!$C37="","",estudianteMateria!$C37)</f>
         <v/>
       </c>
       <c r="C37" s="2" t="str">
-        <f>IF(estudianteMateria!$C37="","",estudianteMateria!$C37)</f>
-        <v/>
-      </c>
-      <c r="D37" s="2" t="str">
-        <f>IF(estudianteMateria!$D37="","",estudianteMateria!$D37)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E37="","",estudianteMateria!$E37)</f>
+        <v/>
+      </c>
+      <c r="D37" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E37" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E37,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F37,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F37" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G37,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H37,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3472,23 +3585,23 @@
         <v/>
       </c>
       <c r="B38" s="2" t="str">
-        <f>IF(estudianteMateria!$B38="","",estudianteMateria!$B38)</f>
+        <f>IF(estudianteMateria!$C38="","",estudianteMateria!$C38)</f>
         <v/>
       </c>
       <c r="C38" s="2" t="str">
-        <f>IF(estudianteMateria!$C38="","",estudianteMateria!$C38)</f>
-        <v/>
-      </c>
-      <c r="D38" s="2" t="str">
-        <f>IF(estudianteMateria!$D38="","",estudianteMateria!$D38)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E38="","",estudianteMateria!$E38)</f>
+        <v/>
+      </c>
+      <c r="D38" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E38" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E38,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F38,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F38" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G38,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H38,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3498,23 +3611,23 @@
         <v/>
       </c>
       <c r="B39" s="2" t="str">
-        <f>IF(estudianteMateria!$B39="","",estudianteMateria!$B39)</f>
+        <f>IF(estudianteMateria!$C39="","",estudianteMateria!$C39)</f>
         <v/>
       </c>
       <c r="C39" s="2" t="str">
-        <f>IF(estudianteMateria!$C39="","",estudianteMateria!$C39)</f>
-        <v/>
-      </c>
-      <c r="D39" s="2" t="str">
-        <f>IF(estudianteMateria!$D39="","",estudianteMateria!$D39)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E39="","",estudianteMateria!$E39)</f>
+        <v/>
+      </c>
+      <c r="D39" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E39" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E39,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F39,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F39" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G39,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H39,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3524,23 +3637,23 @@
         <v/>
       </c>
       <c r="B40" s="2" t="str">
-        <f>IF(estudianteMateria!$B40="","",estudianteMateria!$B40)</f>
+        <f>IF(estudianteMateria!$C40="","",estudianteMateria!$C40)</f>
         <v/>
       </c>
       <c r="C40" s="2" t="str">
-        <f>IF(estudianteMateria!$C40="","",estudianteMateria!$C40)</f>
-        <v/>
-      </c>
-      <c r="D40" s="2" t="str">
-        <f>IF(estudianteMateria!$D40="","",estudianteMateria!$D40)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E40="","",estudianteMateria!$E40)</f>
+        <v/>
+      </c>
+      <c r="D40" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E40" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E40,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F40,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F40" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G40,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H40,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3550,23 +3663,23 @@
         <v/>
       </c>
       <c r="B41" s="2" t="str">
-        <f>IF(estudianteMateria!$B41="","",estudianteMateria!$B41)</f>
+        <f>IF(estudianteMateria!$C41="","",estudianteMateria!$C41)</f>
         <v/>
       </c>
       <c r="C41" s="2" t="str">
-        <f>IF(estudianteMateria!$C41="","",estudianteMateria!$C41)</f>
-        <v/>
-      </c>
-      <c r="D41" s="2" t="str">
-        <f>IF(estudianteMateria!$D41="","",estudianteMateria!$D41)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E41="","",estudianteMateria!$E41)</f>
+        <v/>
+      </c>
+      <c r="D41" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E41" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E41,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F41,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F41" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G41,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H41,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3576,23 +3689,23 @@
         <v/>
       </c>
       <c r="B42" s="2" t="str">
-        <f>IF(estudianteMateria!$B42="","",estudianteMateria!$B42)</f>
+        <f>IF(estudianteMateria!$C42="","",estudianteMateria!$C42)</f>
         <v/>
       </c>
       <c r="C42" s="2" t="str">
-        <f>IF(estudianteMateria!$C42="","",estudianteMateria!$C42)</f>
-        <v/>
-      </c>
-      <c r="D42" s="2" t="str">
-        <f>IF(estudianteMateria!$D42="","",estudianteMateria!$D42)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E42="","",estudianteMateria!$E42)</f>
+        <v/>
+      </c>
+      <c r="D42" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E42" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E42,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F42,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F42" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G42,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H42,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3602,23 +3715,23 @@
         <v/>
       </c>
       <c r="B43" s="2" t="str">
-        <f>IF(estudianteMateria!$B43="","",estudianteMateria!$B43)</f>
+        <f>IF(estudianteMateria!$C43="","",estudianteMateria!$C43)</f>
         <v/>
       </c>
       <c r="C43" s="2" t="str">
-        <f>IF(estudianteMateria!$C43="","",estudianteMateria!$C43)</f>
-        <v/>
-      </c>
-      <c r="D43" s="2" t="str">
-        <f>IF(estudianteMateria!$D43="","",estudianteMateria!$D43)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E43="","",estudianteMateria!$E43)</f>
+        <v/>
+      </c>
+      <c r="D43" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E43" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E43,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F43,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F43" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G43,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H43,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3628,23 +3741,23 @@
         <v/>
       </c>
       <c r="B44" s="2" t="str">
-        <f>IF(estudianteMateria!$B44="","",estudianteMateria!$B44)</f>
+        <f>IF(estudianteMateria!$C44="","",estudianteMateria!$C44)</f>
         <v/>
       </c>
       <c r="C44" s="2" t="str">
-        <f>IF(estudianteMateria!$C44="","",estudianteMateria!$C44)</f>
-        <v/>
-      </c>
-      <c r="D44" s="2" t="str">
-        <f>IF(estudianteMateria!$D44="","",estudianteMateria!$D44)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E44="","",estudianteMateria!$E44)</f>
+        <v/>
+      </c>
+      <c r="D44" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E44" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E44,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F44,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F44" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G44,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H44,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3654,23 +3767,23 @@
         <v/>
       </c>
       <c r="B45" s="2" t="str">
-        <f>IF(estudianteMateria!$B45="","",estudianteMateria!$B45)</f>
+        <f>IF(estudianteMateria!$C45="","",estudianteMateria!$C45)</f>
         <v/>
       </c>
       <c r="C45" s="2" t="str">
-        <f>IF(estudianteMateria!$C45="","",estudianteMateria!$C45)</f>
-        <v/>
-      </c>
-      <c r="D45" s="2" t="str">
-        <f>IF(estudianteMateria!$D45="","",estudianteMateria!$D45)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E45="","",estudianteMateria!$E45)</f>
+        <v/>
+      </c>
+      <c r="D45" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E45" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E45,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F45,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F45" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G45,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H45,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3680,23 +3793,23 @@
         <v/>
       </c>
       <c r="B46" s="2" t="str">
-        <f>IF(estudianteMateria!$B46="","",estudianteMateria!$B46)</f>
+        <f>IF(estudianteMateria!$C46="","",estudianteMateria!$C46)</f>
         <v/>
       </c>
       <c r="C46" s="2" t="str">
-        <f>IF(estudianteMateria!$C46="","",estudianteMateria!$C46)</f>
-        <v/>
-      </c>
-      <c r="D46" s="2" t="str">
-        <f>IF(estudianteMateria!$D46="","",estudianteMateria!$D46)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E46="","",estudianteMateria!$E46)</f>
+        <v/>
+      </c>
+      <c r="D46" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E46" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E46,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F46,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F46" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G46,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H46,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3706,23 +3819,23 @@
         <v/>
       </c>
       <c r="B47" s="2" t="str">
-        <f>IF(estudianteMateria!$B47="","",estudianteMateria!$B47)</f>
+        <f>IF(estudianteMateria!$C47="","",estudianteMateria!$C47)</f>
         <v/>
       </c>
       <c r="C47" s="2" t="str">
-        <f>IF(estudianteMateria!$C47="","",estudianteMateria!$C47)</f>
-        <v/>
-      </c>
-      <c r="D47" s="2" t="str">
-        <f>IF(estudianteMateria!$D47="","",estudianteMateria!$D47)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E47="","",estudianteMateria!$E47)</f>
+        <v/>
+      </c>
+      <c r="D47" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E47" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E47,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F47,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F47" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G47,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H47,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3732,23 +3845,23 @@
         <v/>
       </c>
       <c r="B48" s="2" t="str">
-        <f>IF(estudianteMateria!$B48="","",estudianteMateria!$B48)</f>
+        <f>IF(estudianteMateria!$C48="","",estudianteMateria!$C48)</f>
         <v/>
       </c>
       <c r="C48" s="2" t="str">
-        <f>IF(estudianteMateria!$C48="","",estudianteMateria!$C48)</f>
-        <v/>
-      </c>
-      <c r="D48" s="2" t="str">
-        <f>IF(estudianteMateria!$D48="","",estudianteMateria!$D48)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E48="","",estudianteMateria!$E48)</f>
+        <v/>
+      </c>
+      <c r="D48" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E48" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E48,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F48,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F48" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G48,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H48,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3758,23 +3871,23 @@
         <v/>
       </c>
       <c r="B49" s="2" t="str">
-        <f>IF(estudianteMateria!$B49="","",estudianteMateria!$B49)</f>
+        <f>IF(estudianteMateria!$C49="","",estudianteMateria!$C49)</f>
         <v/>
       </c>
       <c r="C49" s="2" t="str">
-        <f>IF(estudianteMateria!$C49="","",estudianteMateria!$C49)</f>
-        <v/>
-      </c>
-      <c r="D49" s="2" t="str">
-        <f>IF(estudianteMateria!$D49="","",estudianteMateria!$D49)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E49="","",estudianteMateria!$E49)</f>
+        <v/>
+      </c>
+      <c r="D49" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E49" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E49,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F49,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F49" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G49,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H49,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3784,23 +3897,23 @@
         <v/>
       </c>
       <c r="B50" s="2" t="str">
-        <f>IF(estudianteMateria!$B50="","",estudianteMateria!$B50)</f>
+        <f>IF(estudianteMateria!$C50="","",estudianteMateria!$C50)</f>
         <v/>
       </c>
       <c r="C50" s="2" t="str">
-        <f>IF(estudianteMateria!$C50="","",estudianteMateria!$C50)</f>
-        <v/>
-      </c>
-      <c r="D50" s="2" t="str">
-        <f>IF(estudianteMateria!$D50="","",estudianteMateria!$D50)</f>
-        <v/>
+        <f>IF(estudianteMateria!$E50="","",estudianteMateria!$E50)</f>
+        <v/>
+      </c>
+      <c r="D50" s="2" t="e">
+        <f>IF(estudianteMateria!#REF!="","",estudianteMateria!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="E50" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$E50,mod,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$F50,mod,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="F50" s="4" t="str">
-        <f>IFERROR(VLOOKUP(estudianteMateria!$G50,escuelas,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(estudianteMateria!$H50,escuelas,2,FALSE),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>